<commit_message>
Changes to Master in Calculations
</commit_message>
<xml_diff>
--- a/data/nba_win_percent.xlsx
+++ b/data/nba_win_percent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6945849aeec91/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordan/Documents/Coding/INFO-201-Group-1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EA75A6B-5CA3-9F4B-BF06-995B133A1388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36208B40-7D20-6545-9990-DF68AAA922EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{FBBDD081-1019-1E49-83DC-4432AC2FBD5A}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{FBBDD081-1019-1E49-83DC-4432AC2FBD5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -33,97 +27,97 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="31">
   <si>
-    <t>Golden State</t>
+    <t>Start Year</t>
   </si>
   <si>
-    <t>San Antonio</t>
+    <t>Warriors</t>
   </si>
   <si>
-    <t>Cleveland</t>
+    <t>Spurs</t>
   </si>
   <si>
-    <t>Okla City</t>
+    <t>Cavaliers</t>
   </si>
   <si>
-    <t>Toronto</t>
+    <t>Thunder</t>
   </si>
   <si>
-    <t>LA Clippers</t>
+    <t>Raptors</t>
   </si>
   <si>
-    <t>Charlotte</t>
+    <t>Clippers</t>
   </si>
   <si>
-    <t>Miami</t>
+    <t>Hornets</t>
   </si>
   <si>
-    <t>Boston</t>
+    <t>Heat</t>
   </si>
   <si>
-    <t>Atlanta</t>
+    <t>Celtics</t>
   </si>
   <si>
-    <t>Indiana</t>
+    <t>Hawks</t>
   </si>
   <si>
-    <t>Portland</t>
+    <t>Pacers</t>
   </si>
   <si>
-    <t>Chicago</t>
+    <t>Trail Blazers</t>
   </si>
   <si>
-    <t>Detroit</t>
+    <t>Bulls</t>
   </si>
   <si>
-    <t>Washington</t>
+    <t>Pistons</t>
   </si>
   <si>
-    <t>Dallas</t>
+    <t>Wizards</t>
   </si>
   <si>
-    <t>Memphis</t>
+    <t>Mavericks</t>
   </si>
   <si>
-    <t>Utah</t>
+    <t>Grizzlies</t>
   </si>
   <si>
-    <t>Houston</t>
+    <t>Jazz</t>
   </si>
   <si>
-    <t>Orlando</t>
+    <t>Rockets</t>
   </si>
   <si>
-    <t>Milwaukee</t>
+    <t>Magic</t>
   </si>
   <si>
-    <t>Denver</t>
+    <t>Bucks</t>
   </si>
   <si>
-    <t>Sacramento</t>
+    <t>Nuggets</t>
   </si>
   <si>
-    <t>New York</t>
+    <t>Kings</t>
   </si>
   <si>
-    <t>New Orleans</t>
+    <t>Knicks</t>
   </si>
   <si>
-    <t>Minnesota</t>
+    <t>Pelicans</t>
   </si>
   <si>
-    <t>Phoenix</t>
+    <t>Timberwolves</t>
   </si>
   <si>
-    <t>Brooklyn</t>
+    <t>Suns</t>
   </si>
   <si>
-    <t>LA Lakers</t>
+    <t>Nets</t>
   </si>
   <si>
-    <t>Philadelphia</t>
+    <t>Lakers</t>
   </si>
   <si>
-    <t>Start Year</t>
+    <t>76ers</t>
   </si>
 </sst>
 </file>
@@ -502,15 +496,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B1078F-7D4C-B940-986E-3D9EE736034B}">
   <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.2">
@@ -518,7 +512,7 @@
         <v>2015</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>0.83</v>
@@ -544,7 +538,7 @@
         <v>2015</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>0.79300000000000004</v>
@@ -570,7 +564,7 @@
         <v>2015</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
         <v>0.70899999999999996</v>
@@ -596,7 +590,7 @@
         <v>2015</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>0.66</v>
@@ -622,7 +616,7 @@
         <v>2015</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>0.64700000000000002</v>
@@ -648,7 +642,7 @@
         <v>2015</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>0.625</v>
@@ -674,7 +668,7 @@
         <v>2015</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
         <v>0.57299999999999995</v>
@@ -700,7 +694,7 @@
         <v>2015</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
         <v>0.57299999999999995</v>
@@ -726,7 +720,7 @@
         <v>2015</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
         <v>0.56799999999999995</v>
@@ -752,7 +746,7 @@
         <v>2015</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
         <v>0.56499999999999995</v>
@@ -778,7 +772,7 @@
         <v>2015</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
         <v>0.53900000000000003</v>
@@ -804,7 +798,7 @@
         <v>2015</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1">
         <v>0.52700000000000002</v>
@@ -830,7 +824,7 @@
         <v>2015</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
         <v>0.51200000000000001</v>
@@ -856,7 +850,7 @@
         <v>2015</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1">
         <v>0.51200000000000001</v>
@@ -882,7 +876,7 @@
         <v>2015</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1">
         <v>0.5</v>
@@ -908,7 +902,7 @@
         <v>2015</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1">
         <v>0.49399999999999999</v>
@@ -934,7 +928,7 @@
         <v>2015</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1">
         <v>0.48799999999999999</v>
@@ -960,7 +954,7 @@
         <v>2015</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1">
         <v>0.48799999999999999</v>
@@ -986,7 +980,7 @@
         <v>2015</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1">
         <v>0.48299999999999998</v>
@@ -1012,7 +1006,7 @@
         <v>2015</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1">
         <v>0.42699999999999999</v>
@@ -1038,7 +1032,7 @@
         <v>2015</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1">
         <v>0.40200000000000002</v>
@@ -1064,7 +1058,7 @@
         <v>2015</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1">
         <v>0.40200000000000002</v>
@@ -1090,7 +1084,7 @@
         <v>2015</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1">
         <v>0.40200000000000002</v>
@@ -1116,7 +1110,7 @@
         <v>2015</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1">
         <v>0.39</v>
@@ -1142,7 +1136,7 @@
         <v>2015</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
         <v>0.36599999999999999</v>
@@ -1168,7 +1162,7 @@
         <v>2015</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1">
         <v>0.35399999999999998</v>
@@ -1194,7 +1188,7 @@
         <v>2015</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1">
         <v>0.28100000000000003</v>
@@ -1220,7 +1214,7 @@
         <v>2015</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1">
         <v>0.25600000000000001</v>
@@ -1246,7 +1240,7 @@
         <v>2015</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30" s="1">
         <v>0.20699999999999999</v>
@@ -1272,7 +1266,7 @@
         <v>2015</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1">
         <v>0.122</v>
@@ -1298,7 +1292,7 @@
         <v>2014</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
         <v>0.80400000000000005</v>
@@ -1324,7 +1318,7 @@
         <v>2014</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
         <v>0.69399999999999995</v>
@@ -1350,7 +1344,7 @@
         <v>2014</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" s="1">
         <v>0.66300000000000003</v>
@@ -1376,7 +1370,7 @@
         <v>2014</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C35" s="1">
         <v>0.65700000000000003</v>
@@ -1402,7 +1396,7 @@
         <v>2014</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1">
         <v>0.65600000000000003</v>
@@ -1428,7 +1422,7 @@
         <v>2014</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C37" s="1">
         <v>0.65600000000000003</v>
@@ -1454,7 +1448,7 @@
         <v>2014</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" s="1">
         <v>0.65200000000000002</v>
@@ -1480,7 +1474,7 @@
         <v>2014</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C39" s="1">
         <v>0.59799999999999998</v>
@@ -1506,7 +1500,7 @@
         <v>2014</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C40" s="1">
         <v>0.59599999999999997</v>
@@ -1532,7 +1526,7 @@
         <v>2014</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1">
         <v>0.58599999999999997</v>
@@ -1558,7 +1552,7 @@
         <v>2014</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" s="1">
         <v>0.56999999999999995</v>
@@ -1584,7 +1578,7 @@
         <v>2014</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C43" s="1">
         <v>0.56499999999999995</v>
@@ -1610,7 +1604,7 @@
         <v>2014</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" s="1">
         <v>0.54900000000000004</v>
@@ -1636,7 +1630,7 @@
         <v>2014</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C45" s="1">
         <v>0.52300000000000002</v>
@@ -1662,7 +1656,7 @@
         <v>2014</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C46" s="1">
         <v>0.48899999999999999</v>
@@ -1688,7 +1682,7 @@
         <v>2014</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C47" s="1">
         <v>0.47599999999999998</v>
@@ -1714,7 +1708,7 @@
         <v>2014</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C48" s="1">
         <v>0.46500000000000002</v>
@@ -1740,7 +1734,7 @@
         <v>2014</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C49" s="1">
         <v>0.46300000000000002</v>
@@ -1766,7 +1760,7 @@
         <v>2014</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C50" s="1">
         <v>0.46300000000000002</v>
@@ -1792,7 +1786,7 @@
         <v>2014</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C51" s="1">
         <v>0.45500000000000002</v>
@@ -1818,7 +1812,7 @@
         <v>2014</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C52" s="1">
         <v>0.45100000000000001</v>
@@ -1844,7 +1838,7 @@
         <v>2014</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C53" s="1">
         <v>0.40200000000000002</v>
@@ -1870,7 +1864,7 @@
         <v>2014</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C54" s="1">
         <v>0.39</v>
@@ -1896,7 +1890,7 @@
         <v>2014</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C55" s="1">
         <v>0.36599999999999999</v>
@@ -1922,7 +1916,7 @@
         <v>2014</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C56" s="1">
         <v>0.35399999999999998</v>
@@ -1948,7 +1942,7 @@
         <v>2014</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C57" s="1">
         <v>0.30499999999999999</v>
@@ -1974,7 +1968,7 @@
         <v>2014</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C58" s="1">
         <v>0.25600000000000001</v>
@@ -2000,7 +1994,7 @@
         <v>2014</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C59" s="1">
         <v>0.22</v>
@@ -2026,7 +2020,7 @@
         <v>2014</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C60" s="1">
         <v>0.20699999999999999</v>
@@ -2052,7 +2046,7 @@
         <v>2014</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C61" s="1">
         <v>0.19500000000000001</v>
@@ -2078,7 +2072,7 @@
         <v>2013</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C62" s="1">
         <v>0.74</v>
@@ -2104,7 +2098,7 @@
         <v>2013</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C63" s="1">
         <v>0.68300000000000005</v>
@@ -2130,7 +2124,7 @@
         <v>2013</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C64" s="1">
         <v>0.66300000000000003</v>
@@ -2156,7 +2150,7 @@
         <v>2013</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C65" s="1">
         <v>0.66300000000000003</v>
@@ -2182,7 +2176,7 @@
         <v>2013</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C66" s="1">
         <v>0.65300000000000002</v>
@@ -2208,7 +2202,7 @@
         <v>2013</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C67" s="1">
         <v>0.63600000000000001</v>
@@ -2234,7 +2228,7 @@
         <v>2013</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C68" s="1">
         <v>0.63400000000000001</v>
@@ -2260,7 +2254,7 @@
         <v>2013</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69" s="1">
         <v>0.60699999999999998</v>
@@ -2286,7 +2280,7 @@
         <v>2013</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C70" s="1">
         <v>0.59599999999999997</v>
@@ -2312,7 +2306,7 @@
         <v>2013</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C71" s="1">
         <v>0.58499999999999996</v>
@@ -2338,7 +2332,7 @@
         <v>2013</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C72" s="1">
         <v>0.58399999999999996</v>
@@ -2364,7 +2358,7 @@
         <v>2013</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C73" s="1">
         <v>0.57299999999999995</v>
@@ -2390,7 +2384,7 @@
         <v>2013</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C74" s="1">
         <v>0.56299999999999994</v>
@@ -2416,7 +2410,7 @@
         <v>2013</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C75" s="1">
         <v>0.53800000000000003</v>
@@ -2442,7 +2436,7 @@
         <v>2013</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C76" s="1">
         <v>0.52100000000000002</v>
@@ -2468,7 +2462,7 @@
         <v>2013</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C77" s="1">
         <v>0.5</v>
@@ -2494,7 +2488,7 @@
         <v>2013</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C78" s="1">
         <v>0.48799999999999999</v>
@@ -2520,7 +2514,7 @@
         <v>2013</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C79" s="1">
         <v>0.46100000000000002</v>
@@ -2546,7 +2540,7 @@
         <v>2013</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C80" s="1">
         <v>0.45100000000000001</v>
@@ -2572,7 +2566,7 @@
         <v>2013</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C81" s="1">
         <v>0.439</v>
@@ -2598,7 +2592,7 @@
         <v>2013</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C82" s="1">
         <v>0.41499999999999998</v>
@@ -2624,7 +2618,7 @@
         <v>2013</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C83" s="1">
         <v>0.40200000000000002</v>
@@ -2650,7 +2644,7 @@
         <v>2013</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C84" s="1">
         <v>0.35399999999999998</v>
@@ -2676,7 +2670,7 @@
         <v>2013</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C85" s="1">
         <v>0.34200000000000003</v>
@@ -2702,7 +2696,7 @@
         <v>2013</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C86" s="1">
         <v>0.32900000000000001</v>
@@ -2728,7 +2722,7 @@
         <v>2013</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C87" s="1">
         <v>0.30499999999999999</v>
@@ -2754,7 +2748,7 @@
         <v>2013</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C88" s="1">
         <v>0.30499999999999999</v>
@@ -2780,7 +2774,7 @@
         <v>2013</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C89" s="1">
         <v>0.28100000000000003</v>
@@ -2806,7 +2800,7 @@
         <v>2013</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C90" s="1">
         <v>0.23200000000000001</v>
@@ -2832,7 +2826,7 @@
         <v>2013</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C91" s="1">
         <v>0.183</v>
@@ -2858,7 +2852,7 @@
         <v>2012</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C92" s="1">
         <v>0.77900000000000003</v>
@@ -2884,7 +2878,7 @@
         <v>2012</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C93" s="1">
         <v>0.71599999999999997</v>
@@ -2910,7 +2904,7 @@
         <v>2012</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C94" s="1">
         <v>0.69899999999999995</v>
@@ -2936,7 +2930,7 @@
         <v>2012</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C95" s="1">
         <v>0.67</v>
@@ -2962,7 +2956,7 @@
         <v>2012</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C96" s="1">
         <v>0.66</v>
@@ -2988,7 +2982,7 @@
         <v>2012</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C97" s="1">
         <v>0.65900000000000003</v>
@@ -3014,7 +3008,7 @@
         <v>2012</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C98" s="1">
         <v>0.63800000000000001</v>
@@ -3040,7 +3034,7 @@
         <v>2012</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C99" s="1">
         <v>0.6</v>
@@ -3066,7 +3060,7 @@
         <v>2012</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C100" s="1">
         <v>0.58399999999999996</v>
@@ -3092,7 +3086,7 @@
         <v>2012</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101" s="1">
         <v>0.56399999999999995</v>
@@ -3118,7 +3112,7 @@
         <v>2012</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C102" s="1">
         <v>0.53400000000000003</v>
@@ -3144,7 +3138,7 @@
         <v>2012</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C103" s="1">
         <v>0.53200000000000003</v>
@@ -3170,7 +3164,7 @@
         <v>2012</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C104" s="1">
         <v>0.52400000000000002</v>
@@ -3196,7 +3190,7 @@
         <v>2012</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C105" s="1">
         <v>0.52300000000000002</v>
@@ -3222,7 +3216,7 @@
         <v>2012</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C106" s="1">
         <v>0.52300000000000002</v>
@@ -3248,7 +3242,7 @@
         <v>2012</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C107" s="1">
         <v>0.5</v>
@@ -3274,7 +3268,7 @@
         <v>2012</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C108" s="1">
         <v>0.49399999999999999</v>
@@ -3300,7 +3294,7 @@
         <v>2012</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C109" s="1">
         <v>0.442</v>
@@ -3326,7 +3320,7 @@
         <v>2012</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C110" s="1">
         <v>0.41499999999999998</v>
@@ -3352,7 +3346,7 @@
         <v>2012</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C111" s="1">
         <v>0.41499999999999998</v>
@@ -3378,7 +3372,7 @@
         <v>2012</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C112" s="1">
         <v>0.40200000000000002</v>
@@ -3404,7 +3398,7 @@
         <v>2012</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C113" s="1">
         <v>0.378</v>
@@ -3430,7 +3424,7 @@
         <v>2012</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C114" s="1">
         <v>0.35399999999999998</v>
@@ -3456,7 +3450,7 @@
         <v>2012</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C115" s="1">
         <v>0.35399999999999998</v>
@@ -3482,7 +3476,7 @@
         <v>2012</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C116" s="1">
         <v>0.34200000000000003</v>
@@ -3508,7 +3502,7 @@
         <v>2012</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C117" s="1">
         <v>0.32900000000000001</v>
@@ -3534,7 +3528,7 @@
         <v>2012</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C118" s="1">
         <v>0.30499999999999999</v>
@@ -3560,7 +3554,7 @@
         <v>2012</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C119" s="1">
         <v>0.29299999999999998</v>
@@ -3586,7 +3580,7 @@
         <v>2012</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C120" s="1">
         <v>0.25600000000000001</v>
@@ -3612,7 +3606,7 @@
         <v>2012</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C121" s="1">
         <v>0.24399999999999999</v>
@@ -3638,7 +3632,7 @@
         <v>2011</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C122" s="1">
         <v>0.75</v>
@@ -3664,7 +3658,7 @@
         <v>2011</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C123" s="1">
         <v>0.72199999999999998</v>
@@ -3690,7 +3684,7 @@
         <v>2011</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C124" s="1">
         <v>0.70599999999999996</v>
@@ -3716,7 +3710,7 @@
         <v>2011</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C125" s="1">
         <v>0.69299999999999995</v>
@@ -3742,7 +3736,7 @@
         <v>2011</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C126" s="1">
         <v>0.623</v>
@@ -3768,7 +3762,7 @@
         <v>2011</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C127" s="1">
         <v>0.60299999999999998</v>
@@ -3794,7 +3788,7 @@
         <v>2011</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C128" s="1">
         <v>0.59</v>
@@ -3820,7 +3814,7 @@
         <v>2011</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C129" s="1">
         <v>0.58299999999999996</v>
@@ -3846,7 +3840,7 @@
         <v>2011</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C130" s="1">
         <v>0.58099999999999996</v>
@@ -3872,7 +3866,7 @@
         <v>2011</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C131" s="1">
         <v>0.57099999999999995</v>
@@ -3898,7 +3892,7 @@
         <v>2011</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C132" s="1">
         <v>0.56200000000000006</v>
@@ -3924,7 +3918,7 @@
         <v>2011</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C133" s="1">
         <v>0.53500000000000003</v>
@@ -3950,7 +3944,7 @@
         <v>2011</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C134" s="1">
         <v>0.53200000000000003</v>
@@ -3976,7 +3970,7 @@
         <v>2011</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C135" s="1">
         <v>0.52100000000000002</v>
@@ -4002,7 +3996,7 @@
         <v>2011</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C136" s="1">
         <v>0.51500000000000001</v>
@@ -4028,7 +4022,7 @@
         <v>2011</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C137" s="1">
         <v>0.51400000000000001</v>
@@ -4054,7 +4048,7 @@
         <v>2011</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C138" s="1">
         <v>0.51400000000000001</v>
@@ -4080,7 +4074,7 @@
         <v>2011</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C139" s="1">
         <v>0.5</v>
@@ -4106,7 +4100,7 @@
         <v>2011</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C140" s="1">
         <v>0.47</v>
@@ -4132,7 +4126,7 @@
         <v>2011</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C141" s="1">
         <v>0.42399999999999999</v>
@@ -4158,7 +4152,7 @@
         <v>2011</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C142" s="1">
         <v>0.39400000000000002</v>
@@ -4184,7 +4178,7 @@
         <v>2011</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C143" s="1">
         <v>0.379</v>
@@ -4210,7 +4204,7 @@
         <v>2011</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C144" s="1">
         <v>0.34799999999999998</v>
@@ -4236,7 +4230,7 @@
         <v>2011</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C145" s="1">
         <v>0.34799999999999998</v>
@@ -4262,7 +4256,7 @@
         <v>2011</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C146" s="1">
         <v>0.33300000000000002</v>
@@ -4288,7 +4282,7 @@
         <v>2011</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C147" s="1">
         <v>0.33300000000000002</v>
@@ -4314,7 +4308,7 @@
         <v>2011</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C148" s="1">
         <v>0.318</v>
@@ -4340,7 +4334,7 @@
         <v>2011</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C149" s="1">
         <v>0.318</v>
@@ -4366,7 +4360,7 @@
         <v>2011</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C150" s="1">
         <v>0.30299999999999999</v>
@@ -4392,7 +4386,7 @@
         <v>2011</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C151" s="1">
         <v>0.106</v>
@@ -4418,7 +4412,7 @@
         <v>2010</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C152" s="1">
         <v>0.72499999999999998</v>
@@ -4444,7 +4438,7 @@
         <v>2010</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C153" s="1">
         <v>0.71599999999999997</v>
@@ -4470,7 +4464,7 @@
         <v>2010</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C154" s="1">
         <v>0.70599999999999996</v>
@@ -4496,7 +4490,7 @@
         <v>2010</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C155" s="1">
         <v>0.70599999999999996</v>
@@ -4522,7 +4516,7 @@
         <v>2010</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C156" s="1">
         <v>0.67</v>
@@ -4548,7 +4542,7 @@
         <v>2010</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C157" s="1">
         <v>0.66300000000000003</v>
@@ -4574,7 +4568,7 @@
         <v>2010</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C158" s="1">
         <v>0.64600000000000002</v>
@@ -4600,7 +4594,7 @@
         <v>2010</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C159" s="1">
         <v>0.61399999999999999</v>
@@ -4626,7 +4620,7 @@
         <v>2010</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C160" s="1">
         <v>0.58599999999999997</v>
@@ -4652,7 +4646,7 @@
         <v>2010</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C161" s="1">
         <v>0.56799999999999995</v>
@@ -4678,7 +4672,7 @@
         <v>2010</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C162" s="1">
         <v>0.55800000000000005</v>
@@ -4704,7 +4698,7 @@
         <v>2010</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C163" s="1">
         <v>0.54500000000000004</v>
@@ -4730,7 +4724,7 @@
         <v>2010</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C164" s="1">
         <v>0.53200000000000003</v>
@@ -4756,7 +4750,7 @@
         <v>2010</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C165" s="1">
         <v>0.52400000000000002</v>
@@ -4782,7 +4776,7 @@
         <v>2010</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C166" s="1">
         <v>0.48799999999999999</v>
@@ -4808,7 +4802,7 @@
         <v>2010</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C167" s="1">
         <v>0.48799999999999999</v>
@@ -4834,7 +4828,7 @@
         <v>2010</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C168" s="1">
         <v>0.48299999999999998</v>
@@ -4860,7 +4854,7 @@
         <v>2010</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C169" s="1">
         <v>0.47599999999999998</v>
@@ -4886,7 +4880,7 @@
         <v>2010</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C170" s="1">
         <v>0.439</v>
@@ -4912,7 +4906,7 @@
         <v>2010</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C171" s="1">
         <v>0.437</v>
@@ -4938,7 +4932,7 @@
         <v>2010</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C172" s="1">
         <v>0.42699999999999999</v>
@@ -4964,7 +4958,7 @@
         <v>2010</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C173" s="1">
         <v>0.41499999999999998</v>
@@ -4990,7 +4984,7 @@
         <v>2010</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C174" s="1">
         <v>0.39</v>
@@ -5016,7 +5010,7 @@
         <v>2010</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C175" s="1">
         <v>0.36599999999999999</v>
@@ -5042,7 +5036,7 @@
         <v>2010</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C176" s="1">
         <v>0.29299999999999998</v>
@@ -5068,7 +5062,7 @@
         <v>2010</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C177" s="1">
         <v>0.29299999999999998</v>
@@ -5094,7 +5088,7 @@
         <v>2010</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C178" s="1">
         <v>0.28100000000000003</v>
@@ -5120,7 +5114,7 @@
         <v>2010</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C179" s="1">
         <v>0.26800000000000002</v>
@@ -5146,7 +5140,7 @@
         <v>2010</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C180" s="1">
         <v>0.23200000000000001</v>
@@ -5172,7 +5166,7 @@
         <v>2010</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C181" s="1">
         <v>0.20699999999999999</v>

</xml_diff>